<commit_message>
anomali st2023 controller done
</commit_message>
<xml_diff>
--- a/public/data/simdasi/result/Bantaran.xlsx
+++ b/public/data/simdasi/result/Bantaran.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="11" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="15" autoFilterDateGrouping="true" firstSheet="9" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="5.4.3" sheetId="1" r:id="rId4"/>
@@ -19,6 +19,10 @@
     <sheet name="5.4.12" sheetId="10" r:id="rId13"/>
     <sheet name="5.4.13" sheetId="11" r:id="rId14"/>
     <sheet name="5.4.14" sheetId="12" r:id="rId15"/>
+    <sheet name="5.4.15" sheetId="13" r:id="rId16"/>
+    <sheet name="5.4.16" sheetId="14" r:id="rId17"/>
+    <sheet name="5.4.1" sheetId="15" r:id="rId18"/>
+    <sheet name="5.4.2" sheetId="16" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="207">
   <si>
     <t>Luas Panen Tanaman Sayuran dan Buah-buahan Semusim Menurut Jenis Tanaman di Kecamatan Bantaran (ha), 2021– 2022</t>
   </si>
@@ -506,6 +510,147 @@
   </si>
   <si>
     <t>Merpati/Dove</t>
+  </si>
+  <si>
+    <t>Jumlah Rumah Tangga Perikanan Budidaya Menurut Jenis Budidaya di Kecamatan Bantaran, 2022</t>
+  </si>
+  <si>
+    <t>Jumlah Ruta</t>
+  </si>
+  <si>
+    <t>Budidaya Laut/Marine Culture</t>
+  </si>
+  <si>
+    <t>Tambak/Brackish Water Pond</t>
+  </si>
+  <si>
+    <t>Kolam /Fresh Water Pond</t>
+  </si>
+  <si>
+    <t>Keramba/ Cage</t>
+  </si>
+  <si>
+    <t>Jaring Apung/Floating Cage Net</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Jaring Tancap/Step Net</t>
+  </si>
+  <si>
+    <t>Sawah/Paddy Field</t>
+  </si>
+  <si>
+    <t>Produksi Perikanan Tangkap dan Perikanan Budidaya Menurut Subsektor di Kecamatan Bantaran (ton), 2022</t>
+  </si>
+  <si>
+    <t>Jumlah</t>
+  </si>
+  <si>
+    <t>Perikanan Tangkap/Fish Capture</t>
+  </si>
+  <si>
+    <t>Penangkapan Laut/Sea Catching</t>
+  </si>
+  <si>
+    <t>Penangkapan Perairan Umum/ Catching Public Waters</t>
+  </si>
+  <si>
+    <t>Perikanan Budidaya/Aquaculture</t>
+  </si>
+  <si>
+    <t>Tambak/Pond</t>
+  </si>
+  <si>
+    <t>Kolam/Pool</t>
+  </si>
+  <si>
+    <t>0,45</t>
+  </si>
+  <si>
+    <t>Keramba/Cages</t>
+  </si>
+  <si>
+    <t>Jaring Apung/Floating Net</t>
+  </si>
+  <si>
+    <t>Jaring Tancap/Deep Net</t>
+  </si>
+  <si>
+    <t>Sawah/Rice Fields</t>
+  </si>
+  <si>
+    <t>Laut/The Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luas Panen Tanaman Pangan Menurut Jenis Tanaman di Kecamatan Bantaran (ha), 2021–2022 </t>
+  </si>
+  <si>
+    <t>Padi/Paddy</t>
+  </si>
+  <si>
+    <t>Padi Sawah/Paddy In Wet Field</t>
+  </si>
+  <si>
+    <t>Padi Ladang/Paddy In Dry Field</t>
+  </si>
+  <si>
+    <t>Jagung/Maize</t>
+  </si>
+  <si>
+    <t>Kedelai/Soybean</t>
+  </si>
+  <si>
+    <t>Kacang Tanah/Peanut</t>
+  </si>
+  <si>
+    <t>Kacang Hijau/Mungbean</t>
+  </si>
+  <si>
+    <t>Ubi Kayu/Cassava</t>
+  </si>
+  <si>
+    <t>Ubi Jalar/Sweet Potato</t>
+  </si>
+  <si>
+    <t>Produksi Tanaman Pangan Menurut Jenis Tanaman di Kecamatan Bantaran (ton), 2021–2022</t>
+  </si>
+  <si>
+    <t>6 371,99</t>
+  </si>
+  <si>
+    <t>3 728,48</t>
+  </si>
+  <si>
+    <t>2 995,79</t>
+  </si>
+  <si>
+    <t>2 051,78</t>
+  </si>
+  <si>
+    <t>3 376,2</t>
+  </si>
+  <si>
+    <t>1 676,69</t>
+  </si>
+  <si>
+    <t>16 463,02</t>
+  </si>
+  <si>
+    <t>18 037,54</t>
+  </si>
+  <si>
+    <t>43,6</t>
+  </si>
+  <si>
+    <t>25,49</t>
+  </si>
+  <si>
+    <t>18,54</t>
+  </si>
+  <si>
+    <t>3 330,02</t>
   </si>
 </sst>
 </file>
@@ -594,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
@@ -602,6 +747,10 @@
     </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="165" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
@@ -614,7 +763,6 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="165" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,11 +1076,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="31.5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
@@ -1268,13 +1416,13 @@
       <c r="A5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="B5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="5">
         <f>SUM(B5:C5)</f>
         <v>0</v>
       </c>
@@ -1283,13 +1431,13 @@
       <c r="A6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="5">
         <v>8959</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="5">
         <v>12664</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="5">
         <f>SUM(B6:C6)</f>
         <v>21623</v>
       </c>
@@ -1298,13 +1446,13 @@
       <c r="A7" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="B7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="5">
         <f>SUM(B7:C7)</f>
         <v>0</v>
       </c>
@@ -1313,13 +1461,13 @@
       <c r="A8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="5">
         <v>29</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="5">
         <f>SUM(B8:C8)</f>
         <v>29</v>
       </c>
@@ -1328,11 +1476,11 @@
       <c r="A9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="5">
         <v>2033</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5">
         <f>SUM(B9:C9)</f>
         <v>2033</v>
       </c>
@@ -1341,11 +1489,11 @@
       <c r="A10" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="5">
         <v>3237</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5">
         <f>SUM(B10:C10)</f>
         <v>3237</v>
       </c>
@@ -1354,11 +1502,11 @@
       <c r="A11" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11">
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5">
         <f>SUM(B11:C11)</f>
         <v>0</v>
       </c>
@@ -1367,11 +1515,11 @@
       <c r="A12" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="5">
         <v>30</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
         <f>SUM(B12:C12)</f>
         <v>30</v>
       </c>
@@ -1399,8 +1547,8 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1426,7 +1574,7 @@
       <c r="A5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="5">
         <v>1113</v>
       </c>
       <c r="C5"/>
@@ -1435,7 +1583,7 @@
       <c r="A6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="5">
         <v>17000</v>
       </c>
       <c r="C6"/>
@@ -1444,7 +1592,7 @@
       <c r="A7" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="5">
         <v>146000</v>
       </c>
       <c r="C7"/>
@@ -1453,7 +1601,7 @@
       <c r="A8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C8"/>
@@ -1462,7 +1610,7 @@
       <c r="A9" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="5">
         <v>653</v>
       </c>
       <c r="C9"/>
@@ -1471,7 +1619,7 @@
       <c r="A10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="5">
         <v>5000</v>
       </c>
       <c r="C10"/>
@@ -1480,10 +1628,556 @@
       <c r="A11" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="5">
         <v>4670</v>
       </c>
       <c r="C11"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="77.7109375" customWidth="true" style="0"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="83" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18.85546875" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="B5" sqref="B5:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="93.140625" customWidth="true" style="0"/>
+    <col min="2" max="2" width="21" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18.42578125" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1096</v>
+      </c>
+      <c r="C5" s="1">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="1">
+        <v>449</v>
+      </c>
+      <c r="C6" s="1">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="1">
+        <v>647</v>
+      </c>
+      <c r="C7" s="1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4266</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="1">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1ps"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="B5" sqref="B5:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="80.140625" customWidth="true" style="0"/>
+    <col min="2" max="2" width="25.42578125" customWidth="true" style="0"/>
+    <col min="3" max="3" width="25.42578125" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -1520,11 +2214,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="31.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
@@ -1731,11 +2425,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -1874,11 +2568,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -2017,11 +2711,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -2193,11 +2887,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -2369,11 +3063,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -2652,11 +3346,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -2828,11 +3522,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="33.75">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">

</xml_diff>